<commit_message>
Little moves in the ProtoOnly network view
</commit_message>
<xml_diff>
--- a/BySizeAligns.xlsx
+++ b/BySizeAligns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitHubProjects/v6_2018_Network/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitProjects/v6_2018_Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0722AC-AF2D-D14C-B583-A67C15BD02DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776AFAB4-8CA4-554E-82B3-867D457BD758}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="460" windowWidth="29980" windowHeight="26720" activeTab="9" xr2:uid="{A61A643C-678C-5C4A-B0FA-22A61A8A072C}"/>
+    <workbookView xWindow="28800" yWindow="40" windowWidth="28800" windowHeight="16480" activeTab="9" xr2:uid="{A61A643C-678C-5C4A-B0FA-22A61A8A072C}"/>
   </bookViews>
   <sheets>
     <sheet name="8to10" sheetId="2" r:id="rId1"/>
@@ -10646,8 +10646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93117B7-2AF6-0A4A-B4DF-77E51BF42565}">
   <dimension ref="A1:V269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>